<commit_message>
some changes in  add push template
</commit_message>
<xml_diff>
--- a/admin_panel/push_management/add_push_template.xlsx
+++ b/admin_panel/push_management/add_push_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SymlexVPNTestCases\admin_panel\push_management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5C6B50F-E0B2-4BA4-B4DC-2B80DC8DCE81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5DEB0B4-8F0F-4B21-B951-5650176CE03B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="83">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -248,6 +248,39 @@
   </si>
   <si>
     <t>SYM-AP_APT_023</t>
+  </si>
+  <si>
+    <t>SYM-AP_APT_024</t>
+  </si>
+  <si>
+    <t>SYM-AP_APT_025</t>
+  </si>
+  <si>
+    <t>SYM-AP_APT_026</t>
+  </si>
+  <si>
+    <t>enter text, undo, then redo the input action.</t>
+  </si>
+  <si>
+    <t>enter text and navigate through the input field using the Tab key.</t>
+  </si>
+  <si>
+    <t>paste text into the input text field using the paste action.</t>
+  </si>
+  <si>
+    <t>copy and cut text from the input text field.</t>
+  </si>
+  <si>
+    <t>the input is redone, and the field returns to the modified state.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the cursor moves to the next field or element in the expected </t>
+  </si>
+  <si>
+    <t>the pasted text is accepted, and no issues occur.</t>
+  </si>
+  <si>
+    <t>the copied/cut text is successfully performed, and the input is modified accordingly.</t>
   </si>
 </sst>
 </file>
@@ -491,6 +524,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -509,33 +545,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="56">
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
     <dxf>
       <alignment horizontal="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
@@ -585,6 +599,25 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -1130,10 +1163,10 @@
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Test Case ID" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Prerequisites" dataDxfId="5"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Title/Description" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Steps" dataDxfId="0"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Expected result" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Pass / Fail" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Comments" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Steps" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Expected result" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Pass / Fail" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Comments" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Template-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1343,8 +1376,8 @@
   <dimension ref="A1:Z990"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="79" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A27" sqref="A27"/>
+      <pane ySplit="3" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1360,15 +1393,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="24"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="25"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -1390,13 +1423,13 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="25"/>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="27"/>
+      <c r="A2" s="26"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="28"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
@@ -1999,7 +2032,9 @@
       <c r="A18" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="B18" s="10"/>
+      <c r="B18" s="10" t="s">
+        <v>69</v>
+      </c>
       <c r="C18" s="10" t="s">
         <v>46</v>
       </c>
@@ -2035,7 +2070,9 @@
       <c r="A19" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="B19" s="10"/>
+      <c r="B19" s="10" t="s">
+        <v>69</v>
+      </c>
       <c r="C19" s="10" t="s">
         <v>49</v>
       </c>
@@ -2071,7 +2108,9 @@
       <c r="A20" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="B20" s="10"/>
+      <c r="B20" s="10" t="s">
+        <v>69</v>
+      </c>
       <c r="C20" s="10" t="s">
         <v>51</v>
       </c>
@@ -2107,7 +2146,9 @@
       <c r="A21" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="B21" s="10"/>
+      <c r="B21" s="10" t="s">
+        <v>69</v>
+      </c>
       <c r="C21" s="10" t="s">
         <v>55</v>
       </c>
@@ -2143,7 +2184,9 @@
       <c r="A22" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="B22" s="10"/>
+      <c r="B22" s="10" t="s">
+        <v>69</v>
+      </c>
       <c r="C22" s="10" t="s">
         <v>59</v>
       </c>
@@ -2179,7 +2222,9 @@
       <c r="A23" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="B23" s="10"/>
+      <c r="B23" s="10" t="s">
+        <v>69</v>
+      </c>
       <c r="C23" s="10" t="s">
         <v>60</v>
       </c>
@@ -2215,7 +2260,9 @@
       <c r="A24" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="B24" s="10"/>
+      <c r="B24" s="10" t="s">
+        <v>69</v>
+      </c>
       <c r="C24" s="12" t="s">
         <v>62</v>
       </c>
@@ -2251,7 +2298,9 @@
       <c r="A25" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="B25" s="10"/>
+      <c r="B25" s="10" t="s">
+        <v>69</v>
+      </c>
       <c r="C25" s="12" t="s">
         <v>67</v>
       </c>
@@ -2287,12 +2336,18 @@
       <c r="A26" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="B26" s="10"/>
-      <c r="C26" s="12"/>
+      <c r="B26" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>75</v>
+      </c>
       <c r="D26" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="E26" s="12"/>
+      <c r="E26" s="12" t="s">
+        <v>79</v>
+      </c>
       <c r="F26" s="6"/>
       <c r="G26" s="9"/>
       <c r="H26" s="1"/>
@@ -2316,11 +2371,21 @@
       <c r="Z26" s="1"/>
     </row>
     <row r="27" spans="1:26" ht="103.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="14"/>
-      <c r="B27" s="10"/>
-      <c r="C27" s="28"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="12"/>
+      <c r="A27" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C27" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E27" s="12" t="s">
+        <v>80</v>
+      </c>
       <c r="F27" s="6"/>
       <c r="G27" s="9"/>
       <c r="H27" s="1"/>
@@ -2344,11 +2409,21 @@
       <c r="Z27" s="1"/>
     </row>
     <row r="28" spans="1:26" ht="96" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="14"/>
-      <c r="B28" s="10"/>
-      <c r="C28" s="12"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="12"/>
+      <c r="A28" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E28" s="12" t="s">
+        <v>81</v>
+      </c>
       <c r="F28" s="6"/>
       <c r="G28" s="9"/>
       <c r="H28" s="1"/>
@@ -2372,11 +2447,21 @@
       <c r="Z28" s="1"/>
     </row>
     <row r="29" spans="1:26" ht="97.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="14"/>
-      <c r="B29" s="10"/>
-      <c r="C29" s="12"/>
-      <c r="D29" s="10"/>
-      <c r="E29" s="13"/>
+      <c r="A29" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E29" s="13" t="s">
+        <v>82</v>
+      </c>
       <c r="F29" s="6"/>
       <c r="G29" s="9"/>
       <c r="H29" s="1"/>

</xml_diff>

<commit_message>
add tittle and message testcases
</commit_message>
<xml_diff>
--- a/admin_panel/push_management/add_push_template.xlsx
+++ b/admin_panel/push_management/add_push_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SymlexVPNTestCases\admin_panel\push_management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5DEB0B4-8F0F-4B21-B951-5650176CE03B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28EFB2B9-2A78-45E8-973E-65674AEA73AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="81">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -49,28 +49,10 @@
     <t>Expected result</t>
   </si>
   <si>
-    <t>SYM-AP_APT_001</t>
-  </si>
-  <si>
     <t>Test Scenario: add push template</t>
   </si>
   <si>
-    <t>SYM-AP_APT_002</t>
-  </si>
-  <si>
     <t>check with empty text in the template name field</t>
-  </si>
-  <si>
-    <t>SYM-AP_APT_003</t>
-  </si>
-  <si>
-    <t>1. go to admin portal
-2. go to this google and search https://adminportal.symlexvpn.com/vpnadmin/index.php/login/index
-3. login with proper credentials
-4. go to push management 
-5. go to push template
-6. go to add new template
-7. try to check with empty text in the template name field</t>
   </si>
   <si>
     <t>enter a valid and unique template name.</t>
@@ -94,27 +76,6 @@
     <t>the form is submitted successfully</t>
   </si>
   <si>
-    <t>1. go to the admin portal
-2. go to this website https://adminportal.symlexvpn.com/vpnadmin/index.php/login/index
-3. login with credentials
-4. go to push management 
-5. go to push template
-6. go to add new template
-7. try to check with valid text in the template name field</t>
-  </si>
-  <si>
-    <t>SYM-AP_APT_004</t>
-  </si>
-  <si>
-    <t>SYM-AP_APT_005</t>
-  </si>
-  <si>
-    <t>SYM-AP_APT_006</t>
-  </si>
-  <si>
-    <t>SYM-AP_APT_007</t>
-  </si>
-  <si>
     <t>enter only alphabetic characters into the input text field.</t>
   </si>
   <si>
@@ -125,15 +86,6 @@
   </si>
   <si>
     <t>enter a combination of alphabetic and numeric characters.</t>
-  </si>
-  <si>
-    <t>SYM-AP_APT_008</t>
-  </si>
-  <si>
-    <t>SYM-AP_APT_009</t>
-  </si>
-  <si>
-    <t>SYM-AP_APT_010</t>
   </si>
   <si>
     <t>enter special characters into the input text field.</t>
@@ -154,15 +106,6 @@
     <t>enter text with spaces within the content.</t>
   </si>
   <si>
-    <t>SYM-AP_APT_011</t>
-  </si>
-  <si>
-    <t>SYM-AP_APT_012</t>
-  </si>
-  <si>
-    <t>SYM-AP_APT_013</t>
-  </si>
-  <si>
     <t>enter text in uppercase letters.</t>
   </si>
   <si>
@@ -173,9 +116,6 @@
   </si>
   <si>
     <t>enter text with punctuation marks.</t>
-  </si>
-  <si>
-    <t>SYM-AP_APT_014</t>
   </si>
   <si>
     <t>the input is accepted if punctuation marks are allowed; otherwise, an error is displayed</t>
@@ -190,12 +130,6 @@
     <t>attempt to inject HTML or script tags into the input text field.</t>
   </si>
   <si>
-    <t>SYM-AP_APT_015</t>
-  </si>
-  <si>
-    <t>SYM-AP_APT_016</t>
-  </si>
-  <si>
     <t>the input is rejected, and an error message is displayed.</t>
   </si>
   <si>
@@ -203,12 +137,6 @@
   </si>
   <si>
     <t>the input is accepted if emojis are allowed; otherwise, an error is displayed.</t>
-  </si>
-  <si>
-    <t>SYM-AP_APT_017</t>
-  </si>
-  <si>
-    <t>SYM-AP_APT_018</t>
   </si>
   <si>
     <t>enter text with accented characters (e.g., é, ü).</t>
@@ -226,15 +154,6 @@
     <t>the input is cleared, and the field becomes empty.</t>
   </si>
   <si>
-    <t>SYM-AP_APT_019</t>
-  </si>
-  <si>
-    <t>SYM-AP_APT_020</t>
-  </si>
-  <si>
-    <t>SYM-AP_APT_021</t>
-  </si>
-  <si>
     <t>enter text, then undo the input action.</t>
   </si>
   <si>
@@ -244,25 +163,7 @@
     <t>the user is on the "add push template form" page.</t>
   </si>
   <si>
-    <t>SYM-AP_APT_022</t>
-  </si>
-  <si>
-    <t>SYM-AP_APT_023</t>
-  </si>
-  <si>
-    <t>SYM-AP_APT_024</t>
-  </si>
-  <si>
-    <t>SYM-AP_APT_025</t>
-  </si>
-  <si>
-    <t>SYM-AP_APT_026</t>
-  </si>
-  <si>
     <t>enter text, undo, then redo the input action.</t>
-  </si>
-  <si>
-    <t>enter text and navigate through the input field using the Tab key.</t>
   </si>
   <si>
     <t>paste text into the input text field using the paste action.</t>
@@ -281,6 +182,92 @@
   </si>
   <si>
     <t>the copied/cut text is successfully performed, and the input is modified accordingly.</t>
+  </si>
+  <si>
+    <t>enter text and navigate through the input field using the tab key.</t>
+  </si>
+  <si>
+    <t>1. go to  google and search https://adminportal.symlexvpn.com/vpnadmin/index.php/login/index
+2. login with proper credentials
+3. go to push management 
+4. go to push template
+5. go to add new template
+6. try to check with empty text in the template name field</t>
+  </si>
+  <si>
+    <t>SYM-AP_APT_TM_001</t>
+  </si>
+  <si>
+    <t>SYM-AP_APT_TM_002</t>
+  </si>
+  <si>
+    <t>SYM-AP_APT_TM_003</t>
+  </si>
+  <si>
+    <t>SYM-AP_APT_TM_004</t>
+  </si>
+  <si>
+    <t>SYM-AP_APT_TM_005</t>
+  </si>
+  <si>
+    <t>SYM-AP_APT_TM_006</t>
+  </si>
+  <si>
+    <t>SYM-AP_APT_TM_007</t>
+  </si>
+  <si>
+    <t>SYM-AP_APT_TM_008</t>
+  </si>
+  <si>
+    <t>SYM-AP_APT_TM_009</t>
+  </si>
+  <si>
+    <t>SYM-AP_APT_TM_010</t>
+  </si>
+  <si>
+    <t>SYM-AP_APT_TM_012</t>
+  </si>
+  <si>
+    <t>SYM-AP_APT_TM_013</t>
+  </si>
+  <si>
+    <t>SYM-AP_APT_TM_014</t>
+  </si>
+  <si>
+    <t>SYM-AP_APT_TM_015</t>
+  </si>
+  <si>
+    <t>SYM-AP_APT_TM_016</t>
+  </si>
+  <si>
+    <t>SYM-AP_APT_TM_017</t>
+  </si>
+  <si>
+    <t>SYM-AP_APT_TM_018</t>
+  </si>
+  <si>
+    <t>SYM-AP_APT_TM_019</t>
+  </si>
+  <si>
+    <t>SYM-AP_APT_TM_020</t>
+  </si>
+  <si>
+    <t>SYM-AP_APT_TM_021</t>
+  </si>
+  <si>
+    <t>SYM-AP_APT_TM_022</t>
+  </si>
+  <si>
+    <t>SYM-AP_APT_TM_023</t>
+  </si>
+  <si>
+    <t>SYM-AP_APT_TM_024</t>
+  </si>
+  <si>
+    <t>SYM-AP_APT_TM_025</t>
+  </si>
+  <si>
+    <t>SYM-AP_APT_TM_026</t>
   </si>
 </sst>
 </file>
@@ -1376,14 +1363,14 @@
   <dimension ref="A1:Z990"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="79" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C24" sqref="C24"/>
+      <pane ySplit="3" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17" style="15" customWidth="1"/>
-    <col min="2" max="2" width="15.6640625" style="18" customWidth="1"/>
+    <col min="1" max="1" width="21.109375" style="15" customWidth="1"/>
+    <col min="2" max="2" width="21.109375" style="18" customWidth="1"/>
     <col min="3" max="3" width="44.44140625" style="20" customWidth="1"/>
     <col min="4" max="4" width="57.33203125" style="18" customWidth="1"/>
     <col min="5" max="5" width="45.6640625" style="20" customWidth="1"/>
@@ -1394,7 +1381,7 @@
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="23" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" s="24"/>
       <c r="C1" s="24"/>
@@ -1492,21 +1479,21 @@
       <c r="Y3" s="2"/>
       <c r="Z3" s="2"/>
     </row>
-    <row r="4" spans="1:26" ht="131.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:26" ht="120" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>14</v>
+        <v>55</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>6</v>
@@ -1534,21 +1521,21 @@
       <c r="Y4" s="3"/>
       <c r="Z4" s="3"/>
     </row>
-    <row r="5" spans="1:26" ht="136.80000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:26" ht="123" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>15</v>
-      </c>
       <c r="D5" s="10" t="s">
-        <v>22</v>
+        <v>55</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
@@ -1574,19 +1561,19 @@
     </row>
     <row r="6" spans="1:26" ht="87.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
-        <v>13</v>
+        <v>58</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
@@ -1612,19 +1599,19 @@
     </row>
     <row r="7" spans="1:26" ht="81.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
-        <v>23</v>
+        <v>59</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
@@ -1650,19 +1637,19 @@
     </row>
     <row r="8" spans="1:26" ht="85.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
-        <v>24</v>
+        <v>60</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
@@ -1688,19 +1675,19 @@
     </row>
     <row r="9" spans="1:26" ht="79.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
-        <v>25</v>
+        <v>61</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="F9" s="6"/>
       <c r="G9" s="7"/>
@@ -1726,19 +1713,19 @@
     </row>
     <row r="10" spans="1:26" ht="79.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
-        <v>26</v>
+        <v>62</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="F10" s="6"/>
       <c r="G10" s="7"/>
@@ -1764,19 +1751,19 @@
     </row>
     <row r="11" spans="1:26" ht="82.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="F11" s="6"/>
       <c r="G11" s="8"/>
@@ -1802,19 +1789,19 @@
     </row>
     <row r="12" spans="1:26" ht="81" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
-        <v>32</v>
+        <v>63</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="F12" s="6"/>
       <c r="G12" s="8"/>
@@ -1840,19 +1827,19 @@
     </row>
     <row r="13" spans="1:26" ht="87.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="F13" s="6"/>
       <c r="G13" s="8"/>
@@ -1878,19 +1865,19 @@
     </row>
     <row r="14" spans="1:26" ht="80.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
-        <v>40</v>
+        <v>65</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="F14" s="6"/>
       <c r="G14" s="8"/>
@@ -1916,19 +1903,19 @@
     </row>
     <row r="15" spans="1:26" ht="81" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
-        <v>41</v>
+        <v>66</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="F15" s="6"/>
       <c r="G15" s="8"/>
@@ -1954,19 +1941,19 @@
     </row>
     <row r="16" spans="1:26" ht="86.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
-        <v>42</v>
+        <v>67</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="F16" s="6"/>
       <c r="G16" s="8"/>
@@ -1992,19 +1979,19 @@
     </row>
     <row r="17" spans="1:26" ht="96.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
-        <v>47</v>
+        <v>68</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="F17" s="6"/>
       <c r="G17" s="8"/>
@@ -2030,19 +2017,19 @@
     </row>
     <row r="18" spans="1:26" ht="99.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
-        <v>52</v>
+        <v>69</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="F18" s="6"/>
       <c r="G18" s="8"/>
@@ -2068,19 +2055,19 @@
     </row>
     <row r="19" spans="1:26" ht="78.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
-        <v>53</v>
+        <v>70</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="F19" s="6"/>
       <c r="G19" s="8"/>
@@ -2106,19 +2093,19 @@
     </row>
     <row r="20" spans="1:26" ht="84" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="F20" s="6"/>
       <c r="G20" s="8"/>
@@ -2144,19 +2131,19 @@
     </row>
     <row r="21" spans="1:26" ht="87.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="F21" s="6"/>
       <c r="G21" s="8"/>
@@ -2182,19 +2169,19 @@
     </row>
     <row r="22" spans="1:26" ht="96" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="F22" s="6"/>
       <c r="G22" s="8"/>
@@ -2220,19 +2207,19 @@
     </row>
     <row r="23" spans="1:26" ht="82.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>61</v>
+        <v>41</v>
       </c>
       <c r="F23" s="6"/>
       <c r="G23" s="8"/>
@@ -2258,19 +2245,19 @@
     </row>
     <row r="24" spans="1:26" ht="75.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>62</v>
+        <v>42</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>63</v>
+        <v>43</v>
       </c>
       <c r="F24" s="6"/>
       <c r="G24" s="8"/>
@@ -2296,19 +2283,19 @@
     </row>
     <row r="25" spans="1:26" ht="84" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>67</v>
+        <v>44</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>68</v>
+        <v>45</v>
       </c>
       <c r="F25" s="6"/>
       <c r="G25" s="9"/>
@@ -2334,19 +2321,19 @@
     </row>
     <row r="26" spans="1:26" ht="94.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="10" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>75</v>
+        <v>47</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E26" s="12" t="s">
-        <v>79</v>
+        <v>50</v>
       </c>
       <c r="F26" s="6"/>
       <c r="G26" s="9"/>
@@ -2372,19 +2359,19 @@
     </row>
     <row r="27" spans="1:26" ht="103.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="10" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="C27" s="22" t="s">
-        <v>76</v>
+        <v>54</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>80</v>
+        <v>51</v>
       </c>
       <c r="F27" s="6"/>
       <c r="G27" s="9"/>
@@ -2410,19 +2397,19 @@
     </row>
     <row r="28" spans="1:26" ht="96" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="10" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>77</v>
+        <v>48</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>81</v>
+        <v>52</v>
       </c>
       <c r="F28" s="6"/>
       <c r="G28" s="9"/>
@@ -2448,19 +2435,19 @@
     </row>
     <row r="29" spans="1:26" ht="97.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="10" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>78</v>
+        <v>49</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E29" s="13" t="s">
-        <v>82</v>
+        <v>53</v>
       </c>
       <c r="F29" s="6"/>
       <c r="G29" s="9"/>

</xml_diff>